<commit_message>
added add rooms via xls fixed student template
</commit_message>
<xml_diff>
--- a/public/files/template-students.xlsx
+++ b/public/files/template-students.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t xml:space="preserve">NUME</t>
   </si>
@@ -35,6 +35,15 @@
   </si>
   <si>
     <t xml:space="preserve">SEX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Email</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CNP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Telefon</t>
   </si>
 </sst>
 </file>
@@ -144,19 +153,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E210"/>
+  <dimension ref="A1:H210"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
+      <selection pane="topLeft" activeCell="H1" activeCellId="0" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="33.41"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="47.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="26.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="32.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="24.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="29.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="35.43"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="11.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="8.75"/>
   </cols>
   <sheetData>
@@ -175,6 +184,15 @@
       </c>
       <c r="E1" s="1" t="s">
         <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
a lot of fixes added try and catch almost everywhere
</commit_message>
<xml_diff>
--- a/public/files/template-students.xlsx
+++ b/public/files/template-students.xlsx
@@ -20,12 +20,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
-  <si>
-    <t xml:space="preserve">NUME</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PRENUME</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+  <si>
+    <t xml:space="preserve">NUME PRENUME</t>
   </si>
   <si>
     <t xml:space="preserve">MEDIA FINALĂ</t>
@@ -153,20 +150,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H210"/>
+  <dimension ref="A1:G210"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H1" activeCellId="0" sqref="H1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="26.92"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="32.64"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="24.9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="29.56"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="11.6"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="8.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="29.56"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="11.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="8.75"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="28" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -190,9 +186,6 @@
       </c>
       <c r="G1" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>